<commit_message>
Event Summary - regenerate outputs Medicare Records - regenerate outputs Personal Health Records - regenerate outputs Shared Health Summary - regenerate outputs
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/condition-summary-1.xlsx
+++ b/output/SharedHealthSummary/condition-summary-1.xlsx
@@ -833,7 +833,7 @@
     <t>The anatomical location where this condition manifests itself.</t>
   </si>
   <si>
-    <t>Only used if not implicit in code found in Condition.code. If the use case requires attributes from the BodySite resource (e.g. to identify and track separately) then use the standard extension [body-site-instance](https://build.fhir.org/ig/hl7au/au-fhir-base/extension-body-site-instance.html).  May be a summary code, or a reference to a very precise definition of the location, or both.</t>
+    <t>Only used if not implicit in code found in Condition.code. If the use case requires attributes from the BodySite resource (e.g. to identify and track separately) then use the standard extension [body-site-instance](http://hl7.org/fhir/STU3/extension-body-site-instance.html).  May be a summary code, or a reference to a very precise definition of the location, or both.</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1133,7 +1133,7 @@
     <t>Condition.evidence.code</t>
   </si>
   <si>
-    <t xml:space="preserve">Evidence manifestation/symptom </t>
+    <t>Evidence manifestation/symptom</t>
   </si>
   <si>
     <t>A manifestation or symptom that led to the recording of this condition.</t>

</xml_diff>